<commit_message>
train multinomial naive bayes
closes #8
</commit_message>
<xml_diff>
--- a/scores/scores.xlsx
+++ b/scores/scores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Windows-Projects\algos-and-absa\scores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D703B929-A079-44CC-BA24-65D9A3EF709D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B73108A-CC25-4931-856B-BA98A139B7C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{45B9B47C-94F2-4E15-AD76-8F9FCA41D53E}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{45B9B47C-94F2-4E15-AD76-8F9FCA41D53E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="21">
   <si>
     <t>precision</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>~120min</t>
+  </si>
+  <si>
+    <t>multinomal_nb (upsamlping + stratified_split + max_tfidf_features)</t>
+  </si>
+  <si>
+    <t>~10min</t>
   </si>
 </sst>
 </file>
@@ -385,6 +391,24 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="13" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -400,25 +424,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -761,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0D5C6A6-E074-4A99-AE24-B5D766A7B9F9}">
   <dimension ref="A1:F82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,25 +782,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
       <c r="F1" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
       <c r="F2" s="9" t="s">
         <v>17</v>
       </c>
@@ -928,25 +934,25 @@
       <c r="B11" s="3">
         <v>0.88780000000000003</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="14"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="20"/>
     </row>
     <row r="12" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
+      <c r="A12" s="21"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="21"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="15"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
@@ -1077,30 +1083,30 @@
       <c r="B22" s="1">
         <v>0.89319999999999999</v>
       </c>
-      <c r="C22" s="15"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="17"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="12"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
       <c r="F24" s="9" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
@@ -1207,7 +1213,7 @@
         <v>500512</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>8</v>
       </c>
@@ -1224,34 +1230,34 @@
         <v>500512</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B34" s="3">
         <v>0.88780000000000003</v>
       </c>
-      <c r="C34" s="12"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="14"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="18"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="19" t="s">
+      <c r="C34" s="18"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="20"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="21"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B36" s="20"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="21"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="15"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>4</v>
       </c>
@@ -1268,7 +1274,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>11</v>
       </c>
@@ -1285,7 +1291,7 @@
         <v>166838</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>12</v>
       </c>
@@ -1302,7 +1308,7 @@
         <v>166837</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>13</v>
       </c>
@@ -1319,14 +1325,14 @@
         <v>166837</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>6</v>
       </c>
@@ -1339,7 +1345,7 @@
         <v>500512</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>7</v>
       </c>
@@ -1356,7 +1362,7 @@
         <v>500512</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>8</v>
       </c>
@@ -1373,20 +1379,334 @@
         <v>500512</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B45" s="1">
         <v>0.89810000000000001</v>
       </c>
-      <c r="C45" s="15"/>
-      <c r="D45" s="16"/>
-      <c r="E45" s="17"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="12"/>
+    </row>
+    <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="16"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" s="17"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B50" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="C50" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="D50" s="1">
+        <v>0.91</v>
+      </c>
+      <c r="E50" s="1">
+        <v>166837</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B51" s="1">
+        <v>0.69</v>
+      </c>
+      <c r="C51" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="D51" s="1">
+        <v>0.72</v>
+      </c>
+      <c r="E51" s="1">
+        <v>166838</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B52" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="C52" s="1">
+        <v>0.78</v>
+      </c>
+      <c r="D52" s="1">
+        <v>0.76</v>
+      </c>
+      <c r="E52" s="1">
+        <v>166837</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="5"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1">
+        <v>0.79</v>
+      </c>
+      <c r="E54" s="1">
+        <v>500512</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="C55" s="1">
+        <v>0.79</v>
+      </c>
+      <c r="D55" s="1">
+        <v>0.79</v>
+      </c>
+      <c r="E55" s="1">
+        <v>500512</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B56" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="C56" s="1">
+        <v>0.79</v>
+      </c>
+      <c r="D56" s="1">
+        <v>0.79</v>
+      </c>
+      <c r="E56" s="1">
+        <v>500512</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B57" s="3">
+        <v>0.79410000000000003</v>
+      </c>
+      <c r="C57" s="18"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="20"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="21"/>
+      <c r="B58" s="21"/>
+      <c r="C58" s="21"/>
+      <c r="D58" s="21"/>
+      <c r="E58" s="21"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B59" s="14"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="15"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B61" s="1">
+        <v>0.92</v>
+      </c>
+      <c r="C61" s="1">
+        <v>0.91</v>
+      </c>
+      <c r="D61" s="1">
+        <v>0.92</v>
+      </c>
+      <c r="E61" s="1">
+        <v>166838</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B62" s="1">
+        <v>0.64</v>
+      </c>
+      <c r="C62" s="1">
+        <v>0.87</v>
+      </c>
+      <c r="D62" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="E62" s="1">
+        <v>166837</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B63" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C63" s="1">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D63" s="1">
+        <v>0.71</v>
+      </c>
+      <c r="E63" s="1">
+        <v>166837</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="5"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1">
+        <v>0.79</v>
+      </c>
+      <c r="E65" s="1">
+        <v>500512</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B66" s="1">
+        <v>0.82</v>
+      </c>
+      <c r="C66" s="1">
+        <v>0.79</v>
+      </c>
+      <c r="D66" s="1">
+        <v>0.79</v>
+      </c>
+      <c r="E66" s="1">
+        <v>500512</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B67" s="1">
+        <v>0.82</v>
+      </c>
+      <c r="C67" s="1">
+        <v>0.79</v>
+      </c>
+      <c r="D67" s="1">
+        <v>0.79</v>
+      </c>
+      <c r="E67" s="1">
+        <v>500512</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B68" s="1">
+        <v>0.78690000000000004</v>
+      </c>
+      <c r="C68" s="10"/>
+      <c r="D68" s="11"/>
+      <c r="E68" s="12"/>
     </row>
     <row r="82" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="18">
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A59:E59"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="A12:E12"/>
     <mergeCell ref="C45:E45"/>
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A24:E24"/>
@@ -1394,11 +1714,6 @@
     <mergeCell ref="C34:E34"/>
     <mergeCell ref="A35:E35"/>
     <mergeCell ref="A36:E36"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="A12:E12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
train Ridge Classifier model
closes #9
</commit_message>
<xml_diff>
--- a/scores/scores.xlsx
+++ b/scores/scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Windows-Projects\algos-and-absa\scores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B73108A-CC25-4931-856B-BA98A139B7C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB448D3B-F1DA-4E51-B834-4DD7512F2389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{45B9B47C-94F2-4E15-AD76-8F9FCA41D53E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="23">
   <si>
     <t>precision</t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t>~10min</t>
+  </si>
+  <si>
+    <t>ridge_classifier (upsamlping + stratified_split + max_tfidf_features)</t>
+  </si>
+  <si>
+    <t>~20min</t>
   </si>
 </sst>
 </file>
@@ -400,15 +406,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -425,6 +422,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -765,10 +771,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0D5C6A6-E074-4A99-AE24-B5D766A7B9F9}">
-  <dimension ref="A1:F82"/>
+  <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,25 +788,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
       <c r="F1" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
       <c r="F2" s="9" t="s">
         <v>17</v>
       </c>
@@ -934,25 +940,25 @@
       <c r="B11" s="3">
         <v>0.88780000000000003</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="20"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="17"/>
     </row>
     <row r="12" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="15"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="21"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
@@ -1088,25 +1094,25 @@
       <c r="E22" s="12"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
       <c r="F24" s="9" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
@@ -1237,25 +1243,25 @@
       <c r="B34" s="3">
         <v>0.88780000000000003</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="20"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="17"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="21"/>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
+      <c r="A35" s="18"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
+      <c r="A36" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="15"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="21"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
@@ -1391,25 +1397,25 @@
       <c r="E45" s="12"/>
     </row>
     <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="16" t="s">
+      <c r="A47" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B47" s="16"/>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
       <c r="F47" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="17" t="s">
+      <c r="A48" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B48" s="17"/>
-      <c r="C48" s="17"/>
-      <c r="D48" s="17"/>
-      <c r="E48" s="17"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
@@ -1540,25 +1546,25 @@
       <c r="B57" s="3">
         <v>0.79410000000000003</v>
       </c>
-      <c r="C57" s="18"/>
-      <c r="D57" s="19"/>
-      <c r="E57" s="20"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="16"/>
+      <c r="E57" s="17"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="21"/>
-      <c r="B58" s="21"/>
-      <c r="C58" s="21"/>
-      <c r="D58" s="21"/>
-      <c r="E58" s="21"/>
+      <c r="A58" s="18"/>
+      <c r="B58" s="18"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="18"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="13" t="s">
+      <c r="A59" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B59" s="14"/>
-      <c r="C59" s="14"/>
-      <c r="D59" s="14"/>
-      <c r="E59" s="15"/>
+      <c r="B59" s="20"/>
+      <c r="C59" s="20"/>
+      <c r="D59" s="20"/>
+      <c r="E59" s="21"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
@@ -1635,7 +1641,7 @@
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>6</v>
       </c>
@@ -1648,7 +1654,7 @@
         <v>500512</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>7</v>
       </c>
@@ -1665,7 +1671,7 @@
         <v>500512</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>8</v>
       </c>
@@ -1682,7 +1688,7 @@
         <v>500512</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>14</v>
       </c>
@@ -1693,20 +1699,318 @@
       <c r="D68" s="11"/>
       <c r="E68" s="12"/>
     </row>
-    <row r="82" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B70" s="13"/>
+      <c r="C70" s="13"/>
+      <c r="D70" s="13"/>
+      <c r="E70" s="13"/>
+      <c r="F70" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B71" s="14"/>
+      <c r="C71" s="14"/>
+      <c r="D71" s="14"/>
+      <c r="E71" s="14"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B73" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="C73" s="1">
+        <v>1</v>
+      </c>
+      <c r="D73" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="E73" s="1">
+        <v>166837</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B74" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="C74" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="D74" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="E74" s="1">
+        <v>166838</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B75" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="C75" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="D75" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="E75" s="1">
+        <v>166837</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="5"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1">
+        <v>0.89</v>
+      </c>
+      <c r="E77" s="1">
+        <v>500512</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B78" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="C78" s="1">
+        <v>0.89</v>
+      </c>
+      <c r="D78" s="1">
+        <v>0.89</v>
+      </c>
+      <c r="E78" s="1">
+        <v>500512</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B79" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="C79" s="1">
+        <v>0.89</v>
+      </c>
+      <c r="D79" s="1">
+        <v>0.89</v>
+      </c>
+      <c r="E79" s="1">
+        <v>500512</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B80" s="1">
+        <v>0.88480000000000003</v>
+      </c>
+      <c r="C80" s="15"/>
+      <c r="D80" s="16"/>
+      <c r="E80" s="17"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="18"/>
+      <c r="B81" s="18"/>
+      <c r="C81" s="18"/>
+      <c r="D81" s="18"/>
+      <c r="E81" s="18"/>
+    </row>
+    <row r="82" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B82" s="20"/>
+      <c r="C82" s="20"/>
+      <c r="D82" s="20"/>
+      <c r="E82" s="21"/>
+      <c r="F82"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E83" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B84" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="C84" s="1">
+        <v>1</v>
+      </c>
+      <c r="D84" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="E84" s="1">
+        <v>166838</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B85" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="C85" s="1">
+        <v>0.81</v>
+      </c>
+      <c r="D85" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="E85" s="1">
+        <v>166837</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B86" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="C86" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="D86" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="E86" s="1">
+        <v>166837</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="5"/>
+      <c r="B87" s="1"/>
+      <c r="C87" s="1"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B88" s="1"/>
+      <c r="C88" s="1"/>
+      <c r="D88" s="1">
+        <v>0.89</v>
+      </c>
+      <c r="E88" s="1">
+        <v>500512</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B89" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="C89" s="1">
+        <v>0.89</v>
+      </c>
+      <c r="D89" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="E89" s="1">
+        <v>500512</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B90" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="C90" s="1">
+        <v>0.89</v>
+      </c>
+      <c r="D90" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="E90" s="1">
+        <v>500512</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B91" s="1">
+        <v>0.88449999999999995</v>
+      </c>
+      <c r="C91" s="10"/>
+      <c r="D91" s="11"/>
+      <c r="E91" s="12"/>
+    </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="A48:E48"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="A59:E59"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="A12:E12"/>
+  <mergeCells count="24">
+    <mergeCell ref="C91:E91"/>
+    <mergeCell ref="A70:E70"/>
+    <mergeCell ref="A71:E71"/>
+    <mergeCell ref="C80:E80"/>
+    <mergeCell ref="A81:E81"/>
+    <mergeCell ref="A82:E82"/>
     <mergeCell ref="C45:E45"/>
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A24:E24"/>
@@ -1714,6 +2018,17 @@
     <mergeCell ref="C34:E34"/>
     <mergeCell ref="A35:E35"/>
     <mergeCell ref="A36:E36"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A59:E59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
add trained bert-mini and it's scores
closes #6
</commit_message>
<xml_diff>
--- a/scores/scores.xlsx
+++ b/scores/scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Windows-Projects\algos-and-absa\scores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB448D3B-F1DA-4E51-B834-4DD7512F2389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D65798-2DA3-4539-BD27-6389FF6D4E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{45B9B47C-94F2-4E15-AD76-8F9FCA41D53E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="25">
   <si>
     <t>precision</t>
   </si>
@@ -105,6 +105,12 @@
   </si>
   <si>
     <t>~20min</t>
+  </si>
+  <si>
+    <t>bert-mini</t>
+  </si>
+  <si>
+    <t>~240min</t>
   </si>
 </sst>
 </file>
@@ -771,10 +777,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0D5C6A6-E074-4A99-AE24-B5D766A7B9F9}">
-  <dimension ref="A1:F91"/>
+  <dimension ref="A1:F114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="B119" sqref="B119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1997,20 +2003,334 @@
         <v>14</v>
       </c>
       <c r="B91" s="1">
-        <v>0.88449999999999995</v>
+        <v>0.876</v>
       </c>
       <c r="C91" s="10"/>
       <c r="D91" s="11"/>
       <c r="E91" s="12"/>
     </row>
+    <row r="93" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A93" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B93" s="13"/>
+      <c r="C93" s="13"/>
+      <c r="D93" s="13"/>
+      <c r="E93" s="13"/>
+      <c r="F93" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B94" s="14"/>
+      <c r="C94" s="14"/>
+      <c r="D94" s="14"/>
+      <c r="E94" s="14"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B95" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C95" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D95" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E95" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B96" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="C96" s="1">
+        <v>1</v>
+      </c>
+      <c r="D96" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="E96" s="1">
+        <v>166837</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B97" s="1">
+        <v>0.81</v>
+      </c>
+      <c r="C97" s="1">
+        <v>0.82</v>
+      </c>
+      <c r="D97" s="1">
+        <v>0.82</v>
+      </c>
+      <c r="E97" s="1">
+        <v>166838</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B98" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="C98" s="1">
+        <v>0.81</v>
+      </c>
+      <c r="D98" s="1">
+        <v>0.82</v>
+      </c>
+      <c r="E98" s="1">
+        <v>166837</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="5"/>
+      <c r="B99" s="1"/>
+      <c r="C99" s="1"/>
+      <c r="D99" s="1"/>
+      <c r="E99" s="1"/>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B100" s="1"/>
+      <c r="C100" s="1"/>
+      <c r="D100" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="E100" s="1">
+        <v>500512</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B101" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="C101" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="D101" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="E101" s="1">
+        <v>500512</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B102" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="C102" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="D102" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="E102" s="1">
+        <v>500512</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B103" s="1">
+        <v>0.88480000000000003</v>
+      </c>
+      <c r="C103" s="15"/>
+      <c r="D103" s="16"/>
+      <c r="E103" s="17"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="18"/>
+      <c r="B104" s="18"/>
+      <c r="C104" s="18"/>
+      <c r="D104" s="18"/>
+      <c r="E104" s="18"/>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B105" s="20"/>
+      <c r="C105" s="20"/>
+      <c r="D105" s="20"/>
+      <c r="E105" s="21"/>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B106" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C106" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D106" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E106" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B107" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="C107" s="1">
+        <v>1</v>
+      </c>
+      <c r="D107" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="E107" s="1">
+        <v>166838</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B108" s="1">
+        <v>0.86</v>
+      </c>
+      <c r="C108" s="1">
+        <v>0.73</v>
+      </c>
+      <c r="D108" s="1">
+        <v>0.79</v>
+      </c>
+      <c r="E108" s="1">
+        <v>166837</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B109" s="1">
+        <v>0.79</v>
+      </c>
+      <c r="C109" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="D109" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="E109" s="1">
+        <v>166837</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="5"/>
+      <c r="B110" s="1"/>
+      <c r="C110" s="1"/>
+      <c r="D110" s="1"/>
+      <c r="E110" s="1"/>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B111" s="1"/>
+      <c r="C111" s="1"/>
+      <c r="D111" s="1">
+        <v>0.87</v>
+      </c>
+      <c r="E111" s="1">
+        <v>500512</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B112" s="1">
+        <v>0.87</v>
+      </c>
+      <c r="C112" s="1">
+        <v>0.87</v>
+      </c>
+      <c r="D112" s="1">
+        <v>0.87</v>
+      </c>
+      <c r="E112" s="1">
+        <v>500512</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B113" s="1">
+        <v>0.87</v>
+      </c>
+      <c r="C113" s="1">
+        <v>0.87</v>
+      </c>
+      <c r="D113" s="1">
+        <v>0.87</v>
+      </c>
+      <c r="E113" s="1">
+        <v>500512</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B114" s="1">
+        <v>0.86829999999999996</v>
+      </c>
+      <c r="C114" s="10"/>
+      <c r="D114" s="11"/>
+      <c r="E114" s="12"/>
+    </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="C91:E91"/>
-    <mergeCell ref="A70:E70"/>
-    <mergeCell ref="A71:E71"/>
-    <mergeCell ref="C80:E80"/>
-    <mergeCell ref="A81:E81"/>
-    <mergeCell ref="A82:E82"/>
+  <mergeCells count="30">
+    <mergeCell ref="C114:E114"/>
+    <mergeCell ref="A93:E93"/>
+    <mergeCell ref="A94:E94"/>
+    <mergeCell ref="C103:E103"/>
+    <mergeCell ref="A104:E104"/>
+    <mergeCell ref="A105:E105"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A59:E59"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="A12:E12"/>
     <mergeCell ref="C45:E45"/>
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A24:E24"/>
@@ -2018,17 +2338,12 @@
     <mergeCell ref="C34:E34"/>
     <mergeCell ref="A35:E35"/>
     <mergeCell ref="A36:E36"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="A48:E48"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="A59:E59"/>
+    <mergeCell ref="C91:E91"/>
+    <mergeCell ref="A70:E70"/>
+    <mergeCell ref="A71:E71"/>
+    <mergeCell ref="C80:E80"/>
+    <mergeCell ref="A81:E81"/>
+    <mergeCell ref="A82:E82"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>